<commit_message>
worked out bond list from one file
</commit_message>
<xml_diff>
--- a/samples/CLO Holdings 2019.06.28.xlsx
+++ b/samples/CLO Holdings 2019.06.28.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary.lee\China Life Franklin Asset Management\Fixed Income Team - Documents\FI Common\Bond Portfolio data\001 组合持仓情况 - Monthly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\AppData\Local\Programs\Git\git\clamc_trustee\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{8A6939FC-9B77-4FA4-B99A-713EDEB268DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{98F1B5CD-558B-4DC3-9AE4-01EFEDB17E48}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497035A9-EBF9-47AD-90E0-650DCA90C170}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31845" yWindow="2085" windowWidth="20685" windowHeight="13125" xr2:uid="{A53F0594-8544-4865-8456-1C43920F6EA6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A53F0594-8544-4865-8456-1C43920F6EA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum - copy" sheetId="1" r:id="rId1"/>
@@ -45,13 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
-  <si>
-    <t>成本价</t>
-  </si>
-  <si>
-    <t>成本价收益率</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>DE000LB1P2W1</t>
   </si>
@@ -387,6 +381,15 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>Purchase Cost</t>
+  </si>
+  <si>
+    <t>Yield at Cost</t>
   </si>
 </sst>
 </file>
@@ -395,22 +398,22 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="11">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="173" formatCode="&quot;$&quot;#,##0.0"/>
-    <numFmt numFmtId="175" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="180" formatCode="dd\.mm\.yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="dd\.mm\.yy;@"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -418,7 +421,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -437,7 +440,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -451,7 +454,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -518,24 +521,24 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1">
@@ -544,17 +547,17 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="175" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
@@ -566,7 +569,7 @@
     <xf numFmtId="43" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1029,31 +1032,31 @@
       <selection activeCell="W17" sqref="W17"/>
       <selection pane="topRight" activeCell="W17" sqref="W17"/>
       <selection pane="bottomLeft" activeCell="W17" sqref="W17"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="21" customFormat="1" ht="69.599999999999994" customHeight="1">
-      <c r="A1" s="22">
-        <v>43644</v>
+      <c r="A1" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3">
         <v>99.730620248666668</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3">
         <v>103.73068846400001</v>
@@ -1075,7 +1078,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="3">
         <v>100.1262165608108</v>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="3">
         <v>100</v>
@@ -1097,7 +1100,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
         <v>100</v>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3">
         <v>100</v>
@@ -1119,7 +1122,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>99.259</v>
@@ -1130,7 +1133,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3">
         <v>100</v>
@@ -1141,7 +1144,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3">
         <v>100</v>
@@ -1152,7 +1155,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
         <v>100</v>
@@ -1163,7 +1166,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B12" s="3">
         <v>100</v>
@@ -1174,7 +1177,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>129.4398109</v>
@@ -1185,7 +1188,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3">
         <v>109.83808430276832</v>
@@ -1196,7 +1199,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3">
         <v>102.25625149700599</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" s="3">
         <v>100.28854200000001</v>
@@ -1218,7 +1221,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>99.74</v>
@@ -1229,7 +1232,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B18" s="3">
         <v>100</v>
@@ -1240,7 +1243,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3">
         <v>100</v>
@@ -1251,7 +1254,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" s="3">
         <v>99.027000000000001</v>
@@ -1262,7 +1265,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="3">
         <v>98.605800000000002</v>
@@ -1273,7 +1276,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22" s="3">
         <v>100</v>
@@ -1284,7 +1287,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="3">
         <v>99.583483999999999</v>
@@ -1295,7 +1298,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="3">
         <v>100</v>
@@ -1306,7 +1309,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="3">
         <v>100</v>
@@ -1317,7 +1320,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" s="3">
         <v>100</v>
@@ -1328,7 +1331,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="3">
         <v>107.334</v>
@@ -1339,7 +1342,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3">
         <v>130.19216666666668</v>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3">
         <v>107.655</v>
@@ -1361,7 +1364,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3">
         <v>88.051000000000002</v>
@@ -1372,7 +1375,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="3">
         <v>96.201250000000002</v>
@@ -1383,7 +1386,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="3">
         <v>100</v>
@@ -1394,7 +1397,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B33" s="3">
         <v>100.9485</v>
@@ -1405,7 +1408,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" s="3">
         <v>99.397999999999996</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="3">
         <v>104.95</v>
@@ -1427,7 +1430,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" s="3">
         <v>86.144000000000005</v>
@@ -1438,7 +1441,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" s="3">
         <v>117.63514271428572</v>
@@ -1449,7 +1452,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B38" s="3">
         <v>118.33125</v>
@@ -1460,7 +1463,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B39" s="3">
         <v>99.893645448021459</v>
@@ -1471,7 +1474,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B40" s="3">
         <v>99.484999999999999</v>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B41" s="3">
         <v>111.3095491</v>
@@ -1493,7 +1496,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3">
         <v>99.393000000000001</v>
@@ -1504,7 +1507,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B43" s="3">
         <v>104</v>
@@ -1515,7 +1518,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" s="3">
         <v>44.603313200000002</v>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B45" s="3">
         <v>98.231224467499686</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="3">
         <v>39.925874200000003</v>
@@ -1548,7 +1551,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B47" s="3">
         <v>129.774111</v>
@@ -1559,7 +1562,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="3">
         <v>100</v>
@@ -1570,7 +1573,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="3">
         <v>96.278499999999994</v>
@@ -1581,7 +1584,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B50" s="3">
         <v>96.390608999999998</v>
@@ -1592,7 +1595,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B51" s="3">
         <v>135.576649</v>
@@ -1603,7 +1606,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" s="3">
         <v>106.36525</v>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B53" s="3">
         <v>108.47918389473685</v>
@@ -1625,7 +1628,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B54" s="3">
         <v>98.522470642647065</v>
@@ -1636,7 +1639,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B55" s="3">
         <v>100.80617626890756</v>
@@ -1647,7 +1650,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B56" s="3">
         <v>100</v>
@@ -1658,7 +1661,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" s="3">
         <v>98.796999999999997</v>
@@ -1669,7 +1672,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B58" s="3">
         <v>100</v>
@@ -1680,7 +1683,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B59" s="3">
         <v>99.816999999999993</v>
@@ -1691,7 +1694,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B60" s="3">
         <v>86.159044177777773</v>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B61" s="3">
         <v>98.791299899999999</v>
@@ -1713,7 +1716,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B62" s="3">
         <v>84.394499809999985</v>
@@ -1724,7 +1727,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" s="3">
         <v>95.520115000000004</v>
@@ -1735,7 +1738,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B64" s="3">
         <v>99.658000000000001</v>
@@ -1746,7 +1749,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B65" s="3">
         <v>100.0699044173913</v>
@@ -1757,7 +1760,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3">
         <v>99.554000000000002</v>
@@ -1768,7 +1771,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B67" s="3">
         <v>99.578000000000003</v>
@@ -1779,7 +1782,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B68" s="3">
         <v>98.422656416666669</v>
@@ -1790,7 +1793,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B69" s="3">
         <v>95.637958901635869</v>
@@ -1801,7 +1804,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B70" s="3">
         <v>98.233000000000004</v>
@@ -1812,7 +1815,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B71" s="3">
         <v>100</v>
@@ -1823,7 +1826,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3">
         <v>99.104420579185515</v>
@@ -1834,7 +1837,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B73" s="3">
         <v>99.868785000000003</v>
@@ -1845,7 +1848,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B74" s="3">
         <v>100.40769261538462</v>
@@ -1856,7 +1859,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B75" s="3">
         <v>99.031000000000006</v>
@@ -1867,7 +1870,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B76" s="3">
         <v>99.785542239941691</v>
@@ -1878,7 +1881,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B77" s="3">
         <v>99.572999999999993</v>
@@ -1889,7 +1892,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B78" s="3">
         <v>100</v>
@@ -1900,7 +1903,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B79" s="3">
         <v>89.325503665384616</v>
@@ -1911,7 +1914,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B80" s="3">
         <v>96.617999999999995</v>
@@ -1922,7 +1925,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B81" s="3">
         <v>100</v>
@@ -1933,7 +1936,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B82" s="3">
         <v>99.37</v>
@@ -1944,7 +1947,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B83" s="3">
         <v>98.27</v>
@@ -1955,7 +1958,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B84" s="3">
         <v>100</v>
@@ -1966,7 +1969,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85" s="3">
         <v>100</v>
@@ -1977,7 +1980,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3">
         <v>98.436999999999998</v>
@@ -1988,7 +1991,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B87" s="3">
         <v>100</v>
@@ -1999,7 +2002,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B88" s="3">
         <v>100</v>
@@ -2010,7 +2013,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B89" s="3">
         <v>98.474000000000004</v>
@@ -2021,7 +2024,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B90" s="3">
         <v>100</v>
@@ -2032,7 +2035,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B91" s="3">
         <v>99.94666666944444</v>
@@ -2043,7 +2046,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" s="3">
         <v>99.882652857142858</v>
@@ -2054,7 +2057,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B93" s="3">
         <v>100</v>
@@ -2065,7 +2068,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B94" s="3">
         <v>100.10550000000001</v>
@@ -2076,7 +2079,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B95" s="3">
         <v>94.650999999999996</v>
@@ -2087,7 +2090,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B96" s="3">
         <v>100</v>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B97" s="3">
         <v>98.891999999999996</v>
@@ -2109,7 +2112,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3">
         <v>100</v>
@@ -2120,7 +2123,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B99" s="3">
         <v>100</v>
@@ -2131,7 +2134,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B100" s="3">
         <v>100</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B101" s="3">
         <v>98.760103999999998</v>
@@ -2153,7 +2156,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B102" s="3">
         <v>100</v>
@@ -2164,7 +2167,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B103" s="3">
         <v>100</v>
@@ -2175,7 +2178,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B104" s="3">
         <v>100</v>
@@ -2186,7 +2189,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B105" s="3">
         <v>100</v>
@@ -2197,7 +2200,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B106" s="3">
         <v>100</v>
@@ -2208,7 +2211,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B107" s="3">
         <v>99.825000000000003</v>
@@ -2219,7 +2222,7 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B108" s="3">
         <v>99.335999999999999</v>
@@ -2230,7 +2233,7 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B109" s="3">
         <v>100</v>
@@ -2241,7 +2244,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B110" s="3">
         <v>98.96</v>
@@ -2252,7 +2255,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B111" s="3">
         <v>99.231800000000007</v>
@@ -2263,7 +2266,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B112" s="3">
         <v>99.876379</v>
@@ -2860,22 +2863,22 @@
       <c r="E419" s="5"/>
       <c r="F419" s="5"/>
     </row>
-    <row r="420" spans="2:6" ht="15" thickBot="1">
+    <row r="420" spans="2:6" ht="15.75" thickBot="1">
       <c r="B420" s="20">
         <v>1</v>
       </c>
       <c r="C420" s="14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D420" s="5"/>
       <c r="E420" s="5"/>
       <c r="F420" s="5"/>
     </row>
-    <row r="421" spans="2:6" ht="15" thickTop="1">
+    <row r="421" spans="2:6" ht="15.75" thickTop="1">
       <c r="B421" s="19"/>
       <c r="C421" s="14"/>
       <c r="D421" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E421" s="5"/>
       <c r="F421" s="5"/>
@@ -2932,15 +2935,15 @@
       </c>
       <c r="C431" s="14"/>
     </row>
-    <row r="432" spans="2:6" ht="15" thickBot="1">
+    <row r="432" spans="2:6" ht="15.75" thickBot="1">
       <c r="B432" s="20">
         <v>1</v>
       </c>
       <c r="C432" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="433" spans="2:3" ht="15" thickTop="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="433" spans="2:3" ht="15.75" thickTop="1">
       <c r="B433" s="7"/>
       <c r="C433" s="14"/>
     </row>
@@ -3235,6 +3238,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3ABBA213F535143A2153FAFFCD4B404" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de5c07bc042d9b8335c64ae2844aa26e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56ce6572-a240-4cd6-8225-c99230995deb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a3b6e2b5c3108d7449c3295a83331ef" ns2:_="">
     <xsd:import namespace="56ce6572-a240-4cd6-8225-c99230995deb"/>
@@ -3398,15 +3410,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{606202DF-88E4-478A-8FF2-DCCAD82E6ACB}">
   <ds:schemaRefs>
@@ -3424,13 +3427,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B380B56-F354-4B8A-828F-FC89039214C9}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E58CB71-28BD-41E1-AFB4-88B6CEF40785}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B380B56-F354-4B8A-828F-FC89039214C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56ce6572-a240-4cd6-8225-c99230995deb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>